<commit_message>
Updated Maple Tree Generation (full)
</commit_message>
<xml_diff>
--- a/docs/spreadsheets/addedToTheGame.xlsx
+++ b/docs/spreadsheets/addedToTheGame.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tudor\Tudor\010_MCM_MinecraftMod\ArmorTinkersMod_1.18.2\docs\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FC0A2A-6810-4D0F-BAE9-A83894ED0611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F046C113-5623-4D3C-A87B-8F1CF10C78EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="Blocks" sheetId="3" r:id="rId2"/>
-    <sheet name="Effects" sheetId="2" r:id="rId3"/>
+    <sheet name="Loot tables" sheetId="4" r:id="rId3"/>
+    <sheet name="Effects" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="174">
   <si>
     <t>Variable Name</t>
   </si>
@@ -441,6 +443,116 @@
   </si>
   <si>
     <t>VARIANTS-ROT</t>
+  </si>
+  <si>
+    <t>RESIN</t>
+  </si>
+  <si>
+    <t>Resin</t>
+  </si>
+  <si>
+    <t>FUEL</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>MAPLE_LOG</t>
+  </si>
+  <si>
+    <t>Maple Log</t>
+  </si>
+  <si>
+    <t>VARIANTS-AXIS</t>
+  </si>
+  <si>
+    <t>CUBE_COLUMN</t>
+  </si>
+  <si>
+    <t>CUBE_COLUMN, CUBE_COLUMN_HORIZONTAL</t>
+  </si>
+  <si>
+    <t>MAPLE_PLANKS</t>
+  </si>
+  <si>
+    <t>Maple Planks</t>
+  </si>
+  <si>
+    <t>MAPLE_WOOD</t>
+  </si>
+  <si>
+    <t>Maple Wood</t>
+  </si>
+  <si>
+    <t>STRIPPED_MAPLE_LOG</t>
+  </si>
+  <si>
+    <t>STRIPPED_MAPLE_WOOD</t>
+  </si>
+  <si>
+    <t>Stripped Maple Log</t>
+  </si>
+  <si>
+    <t>Stripped Maple Wood</t>
+  </si>
+  <si>
+    <t>IRON AXE</t>
+  </si>
+  <si>
+    <t>STONE AXE</t>
+  </si>
+  <si>
+    <t>maple_logs,
+logs,
+logs_that_burn</t>
+  </si>
+  <si>
+    <t>Loot table name</t>
+  </si>
+  <si>
+    <t>Rolls</t>
+  </si>
+  <si>
+    <t>Entries</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>maple_log</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>2-3 (Uniform)</t>
+  </si>
+  <si>
+    <t>maple_wood</t>
+  </si>
+  <si>
+    <t>Bonus Rolls</t>
+  </si>
+  <si>
+    <t>MAPLE_LEAVES</t>
+  </si>
+  <si>
+    <t>MAPLE SAPLING</t>
+  </si>
+  <si>
+    <t>Maple Leaves</t>
+  </si>
+  <si>
+    <t>Maple Sapling</t>
+  </si>
+  <si>
+    <t>CROSS</t>
+  </si>
+  <si>
+    <t>SAPPLING</t>
+  </si>
+  <si>
+    <t>NO TOOL</t>
   </si>
 </sst>
 </file>
@@ -488,7 +600,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="35">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -578,39 +720,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA636688-6F6C-406D-9BF0-D4B55FCD8666}" name="Tabel1" displayName="Tabel1" ref="A1:I150" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA636688-6F6C-406D-9BF0-D4B55FCD8666}" name="Tabel1" displayName="Tabel1" ref="A1:I150" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A1:I150" xr:uid="{DA636688-6F6C-406D-9BF0-D4B55FCD8666}"/>
   <tableColumns count="9">
-    <tableColumn id="8" xr3:uid="{5C033B63-030D-48E4-B2D7-B1841B77A386}" name="Status" dataDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{F34F146F-5538-4882-B58A-35013A195B90}" name="Variable Name" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{5E61E779-B2D9-4FD8-B397-174A88C30B74}" name="Item Name (en_us.json)" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{A21F2665-CC8B-4588-BA03-8AE7E72E2440}" name="Item Model" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{19FF59F5-DFCE-4F31-BD08-F8AFF8633579}" name="Texture" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{952000D5-3B1E-42F0-8114-A3EC22488D8C}" name="Functionality" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{F5D7D942-246E-4EA3-8BF2-4ECFF0501771}" name="Crafting recipe" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{5F43A53A-05CF-4769-B815-8C7967E962E1}" name="Tooltip" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{5C07AD3B-F118-43D6-945A-6F847A62B389}" name="Creative Tab" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{5C033B63-030D-48E4-B2D7-B1841B77A386}" name="Status" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{F34F146F-5538-4882-B58A-35013A195B90}" name="Variable Name" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{5E61E779-B2D9-4FD8-B397-174A88C30B74}" name="Item Name (en_us.json)" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{A21F2665-CC8B-4588-BA03-8AE7E72E2440}" name="Item Model" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{19FF59F5-DFCE-4F31-BD08-F8AFF8633579}" name="Texture" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{952000D5-3B1E-42F0-8114-A3EC22488D8C}" name="Functionality" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{F5D7D942-246E-4EA3-8BF2-4ECFF0501771}" name="Crafting recipe" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{5F43A53A-05CF-4769-B815-8C7967E962E1}" name="Tooltip" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{5C07AD3B-F118-43D6-945A-6F847A62B389}" name="Creative Tab" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{703966DF-4AE9-4C18-883B-C78EF9CEF18B}" name="Tabel13" displayName="Tabel13" ref="A1:L150" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:L150" xr:uid="{703966DF-4AE9-4C18-883B-C78EF9CEF18B}"/>
-  <tableColumns count="12">
-    <tableColumn id="11" xr3:uid="{8A499605-D65D-4194-9756-0CBBBC3D4ACD}" name="Status" dataDxfId="13"/>
-    <tableColumn id="1" xr3:uid="{E202BD0F-230D-46C6-8979-970A93A577A3}" name="Variable Name" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{5AF3731F-C0BB-41F4-921D-2336FB9DCDB4}" name="Item Name (en_us.json)" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{20FE534B-042C-458E-AD16-A821373BF9E7}" name="Block Item" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{282BDB76-3EF3-4F9E-A87F-D3E671E543CE}" name="Block States" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{DE6D0FE3-F131-4ABA-81B7-D1F794BC9C80}" name="Model" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{EFECA6DA-70D1-499B-845D-83EDCEC51B79}" name="Texture" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{CC0BDB0A-D6A0-47A7-AEF2-85CB59BA369D}" name="Functionality" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{53FE9406-C56B-4FB7-8EDE-EF48C59DCEAA}" name="Crafting recipe" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{9F53C0B9-E9C4-4A32-BDA7-7F6029F77617}" name="Tool" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{C6AA824A-CB33-4994-8F35-A19CD8F48336}" name="Loot Table" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{2F67840D-7286-498B-9C8B-24D163BA5274}" name="Creative Tab" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{703966DF-4AE9-4C18-883B-C78EF9CEF18B}" name="Tabel13" displayName="Tabel13" ref="A1:M150" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:M150" xr:uid="{703966DF-4AE9-4C18-883B-C78EF9CEF18B}"/>
+  <tableColumns count="13">
+    <tableColumn id="11" xr3:uid="{8A499605-D65D-4194-9756-0CBBBC3D4ACD}" name="Status" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{E202BD0F-230D-46C6-8979-970A93A577A3}" name="Variable Name" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{5AF3731F-C0BB-41F4-921D-2336FB9DCDB4}" name="Item Name (en_us.json)" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{20FE534B-042C-458E-AD16-A821373BF9E7}" name="Block Item" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{282BDB76-3EF3-4F9E-A87F-D3E671E543CE}" name="Block States" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{DE6D0FE3-F131-4ABA-81B7-D1F794BC9C80}" name="Model" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{EFECA6DA-70D1-499B-845D-83EDCEC51B79}" name="Texture" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{CC0BDB0A-D6A0-47A7-AEF2-85CB59BA369D}" name="Functionality" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{53FE9406-C56B-4FB7-8EDE-EF48C59DCEAA}" name="Crafting recipe" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{9F53C0B9-E9C4-4A32-BDA7-7F6029F77617}" name="Tool" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{C6AA824A-CB33-4994-8F35-A19CD8F48336}" name="Loot Table" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{2F67840D-7286-498B-9C8B-24D163BA5274}" name="Creative Tab" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{1532E763-CAF2-456E-9FC2-2C9014DC80AA}" name="Tag" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6182B104-5335-4A38-9DD7-3BA31AF626D5}" name="Tabel134" displayName="Tabel134" ref="A1:G150" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G150" xr:uid="{6182B104-5335-4A38-9DD7-3BA31AF626D5}"/>
+  <tableColumns count="7">
+    <tableColumn id="11" xr3:uid="{A8154DDF-62A0-4176-B5BF-1CCE1551093E}" name="Status" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{FBE81043-CED1-4E6F-8F96-0AD1BB800A57}" name="Loot table name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{38EBD6BF-8945-4442-B62F-81F4353B0262}" name="Rolls" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{B26B172C-AE9A-4B93-9BAF-B590A2621439}" name="Bonus Rolls" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{F2CF4A3F-8DF0-488A-9871-6F325CA856C8}" name="Entries" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{519E938C-C475-44A2-A8D3-DED59C6E8DFC}" name="Weight" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{D61B7B34-9B01-44AC-B040-9EE0FC5EFBB6}" name="Count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -879,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,6 +1963,35 @@
         <v>59</v>
       </c>
     </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1815,10 +2003,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5370A7B6-2E7A-435E-B780-54E66613E552}">
-  <dimension ref="A1:L150"/>
+  <dimension ref="A1:M150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,15 +2016,17 @@
     <col min="3" max="3" width="30.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="12" width="9.140625" style="2"/>
+    <col min="13" max="13" width="36.42578125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -1873,8 +2063,11 @@
       <c r="L1" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
@@ -1911,8 +2104,9 @@
       <c r="L2" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -1949,8 +2143,9 @@
       <c r="L3" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>112</v>
       </c>
@@ -1987,8 +2182,9 @@
       <c r="L4" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>112</v>
       </c>
@@ -2025,8 +2221,9 @@
       <c r="L5" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>112</v>
       </c>
@@ -2063,8 +2260,9 @@
       <c r="L6" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -2101,8 +2299,9 @@
       <c r="L7" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>112</v>
       </c>
@@ -2139,8 +2338,9 @@
       <c r="L8" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>112</v>
       </c>
@@ -2177,8 +2377,9 @@
       <c r="L9" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>112</v>
       </c>
@@ -2215,8 +2416,9 @@
       <c r="L10" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>112</v>
       </c>
@@ -2253,8 +2455,9 @@
       <c r="L11" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>112</v>
       </c>
@@ -2291,8 +2494,9 @@
       <c r="L12" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
@@ -2329,8 +2533,9 @@
       <c r="L13" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>112</v>
       </c>
@@ -2367,8 +2572,9 @@
       <c r="L14" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
@@ -2405,8 +2611,9 @@
       <c r="L15" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>112</v>
       </c>
@@ -2443,8 +2650,9 @@
       <c r="L16" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>112</v>
       </c>
@@ -2481,8 +2689,9 @@
       <c r="L17" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
@@ -2519,8 +2728,9 @@
       <c r="L18" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
@@ -2557,8 +2767,9 @@
       <c r="L19" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -2595,8 +2806,9 @@
       <c r="L20" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>112</v>
       </c>
@@ -2633,8 +2845,9 @@
       <c r="L21" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>111</v>
       </c>
@@ -2658,13 +2871,18 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>113</v>
       </c>
@@ -2695,85 +2913,290 @@
       <c r="L23" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2783,8 +3206,9 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2794,8 +3218,9 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2805,8 +3230,9 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2816,8 +3242,9 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2827,8 +3254,9 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2838,8 +3266,9 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2849,8 +3278,9 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-    </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2860,8 +3290,9 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-    </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2871,8 +3302,9 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
-    </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2882,8 +3314,9 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-    </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2893,8 +3326,9 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2904,8 +3338,9 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-    </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2915,8 +3350,9 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-    </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2926,8 +3362,9 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2937,8 +3374,9 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2948,8 +3386,9 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-    </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2959,8 +3398,9 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2970,8 +3410,9 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2981,8 +3422,9 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2992,8 +3434,9 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-    </row>
-    <row r="51" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -3003,8 +3446,9 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
-    </row>
-    <row r="52" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3014,8 +3458,9 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
-    </row>
-    <row r="53" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3025,8 +3470,9 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-    </row>
-    <row r="54" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -3036,8 +3482,9 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -3047,8 +3494,9 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-    </row>
-    <row r="56" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3058,8 +3506,9 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
-    </row>
-    <row r="57" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3069,8 +3518,9 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-    </row>
-    <row r="58" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3080,8 +3530,9 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
-    </row>
-    <row r="59" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M58" s="1"/>
+    </row>
+    <row r="59" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3091,8 +3542,9 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
-    </row>
-    <row r="60" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3102,8 +3554,9 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-    </row>
-    <row r="61" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -3113,8 +3566,9 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
-    </row>
-    <row r="62" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -3124,8 +3578,9 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -3135,8 +3590,9 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-    </row>
-    <row r="64" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -3146,8 +3602,9 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-    </row>
-    <row r="65" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M64" s="1"/>
+    </row>
+    <row r="65" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -3157,8 +3614,9 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M65" s="1"/>
+    </row>
+    <row r="66" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -3168,8 +3626,9 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
-    </row>
-    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M66" s="1"/>
+    </row>
+    <row r="67" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -3179,8 +3638,9 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-    </row>
-    <row r="68" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -3190,8 +3650,9 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
-    </row>
-    <row r="69" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M68" s="1"/>
+    </row>
+    <row r="69" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -3201,8 +3662,9 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
-    </row>
-    <row r="70" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M69" s="1"/>
+    </row>
+    <row r="70" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -3212,8 +3674,9 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
-    </row>
-    <row r="71" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M70" s="1"/>
+    </row>
+    <row r="71" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -3223,8 +3686,9 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
-    </row>
-    <row r="72" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M71" s="1"/>
+    </row>
+    <row r="72" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -3234,8 +3698,9 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
-    </row>
-    <row r="73" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M72" s="1"/>
+    </row>
+    <row r="73" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -3245,8 +3710,9 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
-    </row>
-    <row r="74" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -3256,8 +3722,9 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
-    </row>
-    <row r="75" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3267,8 +3734,9 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
-    </row>
-    <row r="76" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M75" s="1"/>
+    </row>
+    <row r="76" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -3278,8 +3746,9 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
-    </row>
-    <row r="77" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M76" s="1"/>
+    </row>
+    <row r="77" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -3289,8 +3758,9 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M77" s="1"/>
+    </row>
+    <row r="78" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -3300,8 +3770,9 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
-    </row>
-    <row r="79" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M78" s="1"/>
+    </row>
+    <row r="79" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -3311,8 +3782,9 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
-    </row>
-    <row r="80" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M79" s="1"/>
+    </row>
+    <row r="80" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -3322,8 +3794,9 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
-    </row>
-    <row r="81" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M80" s="1"/>
+    </row>
+    <row r="81" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -3333,8 +3806,9 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
-    </row>
-    <row r="82" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M81" s="1"/>
+    </row>
+    <row r="82" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -3344,8 +3818,9 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
-    </row>
-    <row r="83" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -3355,8 +3830,9 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
-    </row>
-    <row r="84" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M83" s="1"/>
+    </row>
+    <row r="84" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -3366,8 +3842,9 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
-    </row>
-    <row r="85" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M84" s="1"/>
+    </row>
+    <row r="85" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -3377,8 +3854,9 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
-    </row>
-    <row r="86" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M85" s="1"/>
+    </row>
+    <row r="86" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -3388,8 +3866,9 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
-    </row>
-    <row r="87" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M86" s="1"/>
+    </row>
+    <row r="87" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -3399,8 +3878,9 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
-    </row>
-    <row r="88" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M87" s="1"/>
+    </row>
+    <row r="88" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -3410,8 +3890,9 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
-    </row>
-    <row r="89" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M88" s="1"/>
+    </row>
+    <row r="89" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
@@ -3421,8 +3902,9 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
-    </row>
-    <row r="90" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M89" s="1"/>
+    </row>
+    <row r="90" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -3432,8 +3914,9 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
-    </row>
-    <row r="91" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M90" s="1"/>
+    </row>
+    <row r="91" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -3443,8 +3926,9 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
-    </row>
-    <row r="92" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M91" s="1"/>
+    </row>
+    <row r="92" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -3454,8 +3938,9 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
-    </row>
-    <row r="93" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M92" s="1"/>
+    </row>
+    <row r="93" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -3465,8 +3950,9 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
-    </row>
-    <row r="94" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M93" s="1"/>
+    </row>
+    <row r="94" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
@@ -3476,8 +3962,9 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
-    </row>
-    <row r="95" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M94" s="1"/>
+    </row>
+    <row r="95" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
@@ -3487,8 +3974,9 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
-    </row>
-    <row r="96" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M95" s="1"/>
+    </row>
+    <row r="96" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -3498,8 +3986,9 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
-    </row>
-    <row r="97" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M96" s="1"/>
+    </row>
+    <row r="97" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -3509,8 +3998,9 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
-    </row>
-    <row r="98" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M97" s="1"/>
+    </row>
+    <row r="98" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -3520,8 +4010,9 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
-    </row>
-    <row r="99" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M98" s="1"/>
+    </row>
+    <row r="99" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -3531,8 +4022,9 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
-    </row>
-    <row r="100" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M99" s="1"/>
+    </row>
+    <row r="100" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -3542,8 +4034,9 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
-    </row>
-    <row r="101" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M100" s="1"/>
+    </row>
+    <row r="101" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -3553,8 +4046,9 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
-    </row>
-    <row r="102" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M101" s="1"/>
+    </row>
+    <row r="102" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -3564,8 +4058,9 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
-    </row>
-    <row r="103" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M102" s="1"/>
+    </row>
+    <row r="103" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
@@ -3575,8 +4070,9 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
-    </row>
-    <row r="104" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M103" s="1"/>
+    </row>
+    <row r="104" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
@@ -3586,8 +4082,9 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
-    </row>
-    <row r="105" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M104" s="1"/>
+    </row>
+    <row r="105" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
@@ -3597,8 +4094,9 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
-    </row>
-    <row r="106" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M105" s="1"/>
+    </row>
+    <row r="106" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -3608,8 +4106,9 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
-    </row>
-    <row r="107" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M106" s="1"/>
+    </row>
+    <row r="107" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -3619,8 +4118,9 @@
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
-    </row>
-    <row r="108" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M107" s="1"/>
+    </row>
+    <row r="108" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -3630,8 +4130,9 @@
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
-    </row>
-    <row r="109" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M108" s="1"/>
+    </row>
+    <row r="109" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -3641,8 +4142,9 @@
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
-    </row>
-    <row r="110" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M109" s="1"/>
+    </row>
+    <row r="110" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -3652,8 +4154,9 @@
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
-    </row>
-    <row r="111" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M110" s="1"/>
+    </row>
+    <row r="111" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -3663,8 +4166,9 @@
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
-    </row>
-    <row r="112" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M111" s="1"/>
+    </row>
+    <row r="112" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -3674,8 +4178,9 @@
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
-    </row>
-    <row r="113" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M112" s="1"/>
+    </row>
+    <row r="113" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -3685,8 +4190,9 @@
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
-    </row>
-    <row r="114" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M113" s="1"/>
+    </row>
+    <row r="114" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -3696,8 +4202,9 @@
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
-    </row>
-    <row r="115" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M114" s="1"/>
+    </row>
+    <row r="115" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -3707,8 +4214,9 @@
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
-    </row>
-    <row r="116" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M115" s="1"/>
+    </row>
+    <row r="116" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -3718,8 +4226,9 @@
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
-    </row>
-    <row r="117" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M116" s="1"/>
+    </row>
+    <row r="117" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -3729,8 +4238,9 @@
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
-    </row>
-    <row r="118" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M117" s="1"/>
+    </row>
+    <row r="118" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -3740,8 +4250,9 @@
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
-    </row>
-    <row r="119" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M118" s="1"/>
+    </row>
+    <row r="119" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -3751,8 +4262,9 @@
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
-    </row>
-    <row r="120" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M119" s="1"/>
+    </row>
+    <row r="120" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -3762,8 +4274,9 @@
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
-    </row>
-    <row r="121" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M120" s="1"/>
+    </row>
+    <row r="121" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -3773,8 +4286,9 @@
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
-    </row>
-    <row r="122" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M121" s="1"/>
+    </row>
+    <row r="122" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -3784,8 +4298,9 @@
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
-    </row>
-    <row r="123" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M122" s="1"/>
+    </row>
+    <row r="123" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -3795,8 +4310,9 @@
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
-    </row>
-    <row r="124" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M123" s="1"/>
+    </row>
+    <row r="124" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -3806,8 +4322,9 @@
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
-    </row>
-    <row r="125" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M124" s="1"/>
+    </row>
+    <row r="125" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -3817,8 +4334,9 @@
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
-    </row>
-    <row r="126" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M125" s="1"/>
+    </row>
+    <row r="126" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -3828,8 +4346,9 @@
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
-    </row>
-    <row r="127" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M126" s="1"/>
+    </row>
+    <row r="127" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -3839,8 +4358,9 @@
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
-    </row>
-    <row r="128" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M127" s="1"/>
+    </row>
+    <row r="128" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -3850,8 +4370,9 @@
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
-    </row>
-    <row r="129" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M128" s="1"/>
+    </row>
+    <row r="129" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -3861,8 +4382,9 @@
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
-    </row>
-    <row r="130" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M129" s="1"/>
+    </row>
+    <row r="130" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -3872,8 +4394,9 @@
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
-    </row>
-    <row r="131" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M130" s="1"/>
+    </row>
+    <row r="131" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -3883,8 +4406,9 @@
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
-    </row>
-    <row r="132" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M131" s="1"/>
+    </row>
+    <row r="132" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -3894,8 +4418,9 @@
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
-    </row>
-    <row r="133" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M132" s="1"/>
+    </row>
+    <row r="133" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -3905,8 +4430,9 @@
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
-    </row>
-    <row r="134" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M133" s="1"/>
+    </row>
+    <row r="134" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
@@ -3916,8 +4442,9 @@
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
-    </row>
-    <row r="135" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M134" s="1"/>
+    </row>
+    <row r="135" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -3927,8 +4454,9 @@
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
-    </row>
-    <row r="136" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M135" s="1"/>
+    </row>
+    <row r="136" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -3938,8 +4466,9 @@
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
-    </row>
-    <row r="137" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M136" s="1"/>
+    </row>
+    <row r="137" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -3949,8 +4478,9 @@
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
-    </row>
-    <row r="138" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M137" s="1"/>
+    </row>
+    <row r="138" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -3960,8 +4490,9 @@
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
-    </row>
-    <row r="139" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M138" s="1"/>
+    </row>
+    <row r="139" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -3971,8 +4502,9 @@
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
-    </row>
-    <row r="140" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M139" s="1"/>
+    </row>
+    <row r="140" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -3982,8 +4514,9 @@
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
-    </row>
-    <row r="141" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M140" s="1"/>
+    </row>
+    <row r="141" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -3993,8 +4526,9 @@
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
-    </row>
-    <row r="142" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M141" s="1"/>
+    </row>
+    <row r="142" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
@@ -4004,8 +4538,9 @@
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
-    </row>
-    <row r="143" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M142" s="1"/>
+    </row>
+    <row r="143" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
@@ -4015,8 +4550,9 @@
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
-    </row>
-    <row r="144" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M143" s="1"/>
+    </row>
+    <row r="144" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
@@ -4026,8 +4562,9 @@
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
-    </row>
-    <row r="145" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M144" s="1"/>
+    </row>
+    <row r="145" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -4037,8 +4574,9 @@
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
-    </row>
-    <row r="146" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M145" s="1"/>
+    </row>
+    <row r="146" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
@@ -4048,8 +4586,9 @@
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
-    </row>
-    <row r="147" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M146" s="1"/>
+    </row>
+    <row r="147" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
@@ -4059,8 +4598,9 @@
       <c r="J147" s="1"/>
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
-    </row>
-    <row r="148" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M147" s="1"/>
+    </row>
+    <row r="148" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
@@ -4070,8 +4610,9 @@
       <c r="J148" s="1"/>
       <c r="K148" s="1"/>
       <c r="L148" s="1"/>
-    </row>
-    <row r="149" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M148" s="1"/>
+    </row>
+    <row r="149" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
@@ -4081,8 +4622,9 @@
       <c r="J149" s="1"/>
       <c r="K149" s="1"/>
       <c r="L149" s="1"/>
-    </row>
-    <row r="150" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M149" s="1"/>
+    </row>
+    <row r="150" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
@@ -4092,6 +4634,7 @@
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
       <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4102,6 +4645,850 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F571EFCD-24EF-4623-80D6-66EA66B261E5}">
+  <dimension ref="A1:G150"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="14.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+    </row>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+    </row>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+    </row>
+    <row r="102" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+    </row>
+    <row r="103" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+    </row>
+    <row r="104" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+    </row>
+    <row r="105" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+    </row>
+    <row r="106" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+    </row>
+    <row r="107" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+    </row>
+    <row r="108" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+    </row>
+    <row r="109" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+    </row>
+    <row r="111" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+    </row>
+    <row r="112" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+    </row>
+    <row r="113" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+    </row>
+    <row r="114" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+    </row>
+    <row r="115" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+    </row>
+    <row r="116" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+    </row>
+    <row r="117" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+    </row>
+    <row r="118" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+    </row>
+    <row r="119" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+    </row>
+    <row r="120" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+    </row>
+    <row r="121" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+    </row>
+    <row r="122" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+    </row>
+    <row r="123" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+    </row>
+    <row r="124" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+    </row>
+    <row r="125" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+    </row>
+    <row r="126" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+    </row>
+    <row r="127" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+    </row>
+    <row r="128" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+    </row>
+    <row r="129" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+    </row>
+    <row r="130" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+    </row>
+    <row r="131" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+    </row>
+    <row r="132" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+    </row>
+    <row r="133" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+    </row>
+    <row r="134" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+    </row>
+    <row r="135" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+    </row>
+    <row r="136" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+    </row>
+    <row r="137" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+    </row>
+    <row r="138" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+    </row>
+    <row r="139" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+    </row>
+    <row r="140" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+    </row>
+    <row r="141" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+    </row>
+    <row r="142" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+    </row>
+    <row r="143" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+    </row>
+    <row r="144" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+    </row>
+    <row r="145" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1"/>
+    </row>
+    <row r="146" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+    </row>
+    <row r="147" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E147" s="1"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+    </row>
+    <row r="148" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+    </row>
+    <row r="149" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+    </row>
+    <row r="150" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D2B0C4-1CEA-4032-B91B-FF8661DE2CBD}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>